<commit_message>
Adding EB automation using appium
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Config_Ruby.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Config_Ruby.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="78">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -856,16 +856,12 @@
 validate_Result=1. Initial start_path value: : /app/Configtest/specRunner.html
 validate_Result=2. After setting new start_path value: : /app/index.html
 };</t>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -1300,18 +1296,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="8.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="37.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="6.02265625" collapsed="true"/>
+    <col min="1" max="1" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="37.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="6" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="35.25" thickBot="1">
@@ -1373,9 +1367,7 @@
       <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" ht="214.5" thickBot="1">
@@ -1400,9 +1392,7 @@
         <v>74</v>
       </c>
       <c r="I3" s="2"/>
-      <c r="J3" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="225.75" thickBot="1">
@@ -1427,9 +1417,7 @@
         <v>75</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" ht="169.5" thickBot="1">
@@ -1479,9 +1467,7 @@
         <v>77</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" ht="214.5" thickBot="1">
@@ -1506,9 +1492,7 @@
         <v>55</v>
       </c>
       <c r="I7" s="2"/>
-      <c r="J7" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" ht="203.25" thickBot="1">
@@ -1533,9 +1517,7 @@
         <v>56</v>
       </c>
       <c r="I8" s="2"/>
-      <c r="J8" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" ht="214.5" thickBot="1">
@@ -1560,9 +1542,7 @@
         <v>57</v>
       </c>
       <c r="I9" s="2"/>
-      <c r="J9" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" ht="203.25" thickBot="1">
@@ -1612,9 +1592,7 @@
         <v>59</v>
       </c>
       <c r="I11" s="2"/>
-      <c r="J11" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11" ht="214.5" thickBot="1">
@@ -1639,9 +1617,7 @@
         <v>60</v>
       </c>
       <c r="I12" s="2"/>
-      <c r="J12" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="225.75" thickBot="1">
@@ -1666,9 +1642,7 @@
         <v>61</v>
       </c>
       <c r="I13" s="2"/>
-      <c r="J13" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="214.5" thickBot="1">
@@ -1718,9 +1692,7 @@
         <v>63</v>
       </c>
       <c r="I15" s="2"/>
-      <c r="J15" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="203.25" thickBot="1">
@@ -1745,9 +1717,7 @@
         <v>64</v>
       </c>
       <c r="I16" s="2"/>
-      <c r="J16" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" ht="203.25" thickBot="1">
@@ -1772,9 +1742,7 @@
         <v>65</v>
       </c>
       <c r="I17" s="2"/>
-      <c r="J17" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" ht="192" thickBot="1">
@@ -1799,9 +1767,7 @@
         <v>66</v>
       </c>
       <c r="I18" s="2"/>
-      <c r="J18" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="214.5" thickBot="1">
@@ -1826,9 +1792,7 @@
         <v>67</v>
       </c>
       <c r="I19" s="2"/>
-      <c r="J19" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="214.5" thickBot="1">
@@ -1853,9 +1817,7 @@
         <v>68</v>
       </c>
       <c r="I20" s="2"/>
-      <c r="J20" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" ht="203.25" thickBot="1">
@@ -1880,9 +1842,7 @@
         <v>69</v>
       </c>
       <c r="I21" s="2"/>
-      <c r="J21" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" ht="192" thickBot="1">
@@ -1907,9 +1867,7 @@
         <v>70</v>
       </c>
       <c r="I22" s="2"/>
-      <c r="J22" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" ht="225.75" thickBot="1">
@@ -1934,9 +1892,7 @@
         <v>71</v>
       </c>
       <c r="I23" s="2"/>
-      <c r="J23" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11" ht="214.5" thickBot="1">

</xml_diff>